<commit_message>
edit player loop bug fix
</commit_message>
<xml_diff>
--- a/team_data/Chennai_SouthAfrica/Chennai_SouthAfrica.xlsx
+++ b/team_data/Chennai_SouthAfrica/Chennai_SouthAfrica.xlsx
@@ -1,26 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\IIT\1st Year\1st Trimester\CM1601 [PRO]  Programming Fundamentals\Course Work\team_data\Chennai_SouthAfrica\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B11C628-0541-4C93-A6A6-07A411EC6652}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="4425" windowWidth="15375" windowHeight="12525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="20">
+  <si>
+    <t>PLAYER NAME</t>
+  </si>
   <si>
     <t>Runs</t>
   </si>
@@ -37,13 +34,16 @@
     <t>Batting Order</t>
   </si>
   <si>
+    <t>PLAYER NUMBER</t>
+  </si>
+  <si>
     <t>Temba Bavuma(C)</t>
   </si>
   <si>
     <t>Quinton de Kock</t>
   </si>
   <si>
-    <t>Rassie Va der Dussen</t>
+    <t>ranjan ramanayake</t>
   </si>
   <si>
     <t>Aiden Markram</t>
@@ -73,14 +73,14 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>PLAYER NAME</t>
+    <t>aa</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -143,14 +143,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -197,7 +189,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -229,27 +221,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -281,24 +255,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -474,38 +430,39 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -514,18 +471,21 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -534,18 +494,18 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -554,18 +514,18 @@
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -574,18 +534,18 @@
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -594,18 +554,18 @@
         <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E6" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F6">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -614,18 +574,18 @@
         <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E7" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F7">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -634,18 +594,18 @@
         <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F8">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -654,18 +614,18 @@
         <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E9" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F9">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -674,18 +634,18 @@
         <v>0</v>
       </c>
       <c r="D10" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E10" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F10">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -694,18 +654,18 @@
         <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E11" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F11">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -714,10 +674,10 @@
         <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E12" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F12">
         <v>11</v>

</xml_diff>

<commit_message>
points table index removed
</commit_message>
<xml_diff>
--- a/team_data/Chennai_SouthAfrica/Chennai_SouthAfrica.xlsx
+++ b/team_data/Chennai_SouthAfrica/Chennai_SouthAfrica.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\IIT\1st Year\1st Trimester\CM1601 [PRO]  Programming Fundamentals\Course Work\team_data\Chennai_SouthAfrica\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{159282B9-1290-42B0-BCDC-965FECA2B3C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="28680" yWindow="6810" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="18">
   <si>
     <t>PLAYER NAME</t>
   </si>
@@ -34,18 +40,12 @@
     <t>Batting Order</t>
   </si>
   <si>
-    <t>PLAYER NUMBER</t>
-  </si>
-  <si>
     <t>Temba Bavuma(C)</t>
   </si>
   <si>
     <t>Quinton de Kock</t>
   </si>
   <si>
-    <t>ranjan ramanayake</t>
-  </si>
-  <si>
     <t>Aiden Markram</t>
   </si>
   <si>
@@ -73,14 +73,14 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>aa</t>
+    <t>Rassie Van der Dussen</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -143,6 +143,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -189,7 +197,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -221,9 +229,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -255,6 +281,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -430,14 +474,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -456,14 +505,11 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
       <c r="B2">
         <v>0</v>
       </c>
@@ -471,21 +517,18 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
-      <c r="G2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -494,18 +537,18 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -514,18 +557,18 @@
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -534,18 +577,18 @@
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -554,18 +597,18 @@
         <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F6">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -574,18 +617,18 @@
         <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F7">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -594,18 +637,18 @@
         <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F8">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -614,18 +657,18 @@
         <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F9">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -634,18 +677,18 @@
         <v>0</v>
       </c>
       <c r="D10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F10">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -654,18 +697,18 @@
         <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F11">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -674,10 +717,10 @@
         <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F12">
         <v>11</v>

</xml_diff>

<commit_message>
duplicate match issue fixed
</commit_message>
<xml_diff>
--- a/team_data/Chennai_SouthAfrica/Chennai_SouthAfrica.xlsx
+++ b/team_data/Chennai_SouthAfrica/Chennai_SouthAfrica.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\IIT\1st Year\1st Trimester\CM1601 [PRO]  Programming Fundamentals\Course Work\team_data\Chennai_SouthAfrica\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{159282B9-1290-42B0-BCDC-965FECA2B3C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="6810" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -46,6 +40,9 @@
     <t>Quinton de Kock</t>
   </si>
   <si>
+    <t>Rassie Van der Dussen</t>
+  </si>
+  <si>
     <t>Aiden Markram</t>
   </si>
   <si>
@@ -71,16 +68,13 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>Rassie Van der Dussen</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -143,14 +137,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -197,7 +183,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -229,27 +215,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -281,24 +249,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -474,19 +424,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="18.85546875" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -506,7 +451,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -517,16 +462,16 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -537,18 +482,18 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -557,18 +502,18 @@
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -577,18 +522,18 @@
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -597,18 +542,18 @@
         <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F6">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -617,18 +562,18 @@
         <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F7">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -637,18 +582,18 @@
         <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F8">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -657,18 +602,18 @@
         <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F9">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -677,18 +622,18 @@
         <v>0</v>
       </c>
       <c r="D10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F10">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -697,18 +642,18 @@
         <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F11">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -717,10 +662,10 @@
         <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E12" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F12">
         <v>11</v>

</xml_diff>